<commit_message>
ultimos cambios por ahora
</commit_message>
<xml_diff>
--- a/RA_SEPIA_V1-SinData.xlsx
+++ b/RA_SEPIA_V1-SinData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B2326A-6E3C-439D-80B1-9742121ECB53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90834F1D-D582-4588-BEF6-E5CACE383920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <r>
       <rPr>
@@ -171,6 +171,15 @@
   </si>
   <si>
     <t>Samuel Martinez Sanchez</t>
+  </si>
+  <si>
+    <t>cealvearm@correo.usbcali.edu.co</t>
+  </si>
+  <si>
+    <t>carlosalvear@gmail.com</t>
+  </si>
+  <si>
+    <t>Carlos Eduardo Alvear Mutis</t>
   </si>
 </sst>
 </file>
@@ -1320,14 +1329,28 @@
       <c r="P19" s="24"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="46"/>
+      <c r="A20" s="7">
+        <v>3</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="7">
+        <v>30000070033</v>
+      </c>
+      <c r="D20" s="59" t="s">
+        <v>36</v>
+      </c>
       <c r="E20" s="47"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="10"/>
+      <c r="F20" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="7">
+        <v>3208928893</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>38</v>
+      </c>
       <c r="I20" s="13"/>
       <c r="J20" s="14"/>
       <c r="K20" s="19"/>
@@ -2461,8 +2484,10 @@
     <hyperlink ref="D14" r:id="rId2" xr:uid="{F548C158-A83B-4062-BF97-7A2873D64386}"/>
     <hyperlink ref="D17" r:id="rId3" xr:uid="{DCF3FAB9-7C3B-415D-AA64-01DF87A6487D}"/>
     <hyperlink ref="F17" r:id="rId4" xr:uid="{6886C738-862A-440F-97A4-66DAC27C2D7D}"/>
+    <hyperlink ref="D20" r:id="rId5" xr:uid="{0652A18D-9FBA-4762-8946-76B86A16A7DD}"/>
+    <hyperlink ref="F20" r:id="rId6" xr:uid="{9154B9CF-0A7D-47B9-BF3F-36CB9C46D840}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId5"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "ultimos cambios por ahora"
This reverts commit 60a46a4aab0cffa4e28d33830a26cc4c68538c64.
</commit_message>
<xml_diff>
--- a/RA_SEPIA_V1-SinData.xlsx
+++ b/RA_SEPIA_V1-SinData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90834F1D-D582-4588-BEF6-E5CACE383920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B2326A-6E3C-439D-80B1-9742121ECB53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
   <si>
     <r>
       <rPr>
@@ -171,15 +171,6 @@
   </si>
   <si>
     <t>Samuel Martinez Sanchez</t>
-  </si>
-  <si>
-    <t>cealvearm@correo.usbcali.edu.co</t>
-  </si>
-  <si>
-    <t>carlosalvear@gmail.com</t>
-  </si>
-  <si>
-    <t>Carlos Eduardo Alvear Mutis</t>
   </si>
 </sst>
 </file>
@@ -1329,28 +1320,14 @@
       <c r="P19" s="24"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
-        <v>3</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="7">
-        <v>30000070033</v>
-      </c>
-      <c r="D20" s="59" t="s">
-        <v>36</v>
-      </c>
+      <c r="A20" s="7"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="46"/>
       <c r="E20" s="47"/>
-      <c r="F20" s="60" t="s">
-        <v>37</v>
-      </c>
-      <c r="G20" s="7">
-        <v>3208928893</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>38</v>
-      </c>
+      <c r="F20" s="10"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="10"/>
       <c r="I20" s="13"/>
       <c r="J20" s="14"/>
       <c r="K20" s="19"/>
@@ -2484,10 +2461,8 @@
     <hyperlink ref="D14" r:id="rId2" xr:uid="{F548C158-A83B-4062-BF97-7A2873D64386}"/>
     <hyperlink ref="D17" r:id="rId3" xr:uid="{DCF3FAB9-7C3B-415D-AA64-01DF87A6487D}"/>
     <hyperlink ref="F17" r:id="rId4" xr:uid="{6886C738-862A-440F-97A4-66DAC27C2D7D}"/>
-    <hyperlink ref="D20" r:id="rId5" xr:uid="{0652A18D-9FBA-4762-8946-76B86A16A7DD}"/>
-    <hyperlink ref="F20" r:id="rId6" xr:uid="{9154B9CF-0A7D-47B9-BF3F-36CB9C46D840}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId7"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cadena de conexion y guardar en la base de datos implementado, mas arreglo de bugs
</commit_message>
<xml_diff>
--- a/RA_SEPIA_V1-SinData.xlsx
+++ b/RA_SEPIA_V1-SinData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3471F4E-2EB0-4EE7-8C20-AFA043F8145C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{A3471F4E-2EB0-4EE7-8C20-AFA043F8145C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5BB5634-C232-4039-988B-9C6BE6E0EB36}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3765" yWindow="3765" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -422,6 +422,99 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -440,120 +533,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -645,9 +645,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -685,9 +685,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -720,9 +720,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -755,9 +772,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -933,11 +967,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q76"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A57" zoomScale="73" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65:C67"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68:Q68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" customWidth="1"/>
     <col min="2" max="2" width="6.85546875" customWidth="1"/>
@@ -958,259 +992,259 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="22" t="s">
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="23" t="s">
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="53"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="55"/>
+      <c r="M9" s="55"/>
+      <c r="N9" s="55"/>
+      <c r="O9" s="55"/>
+      <c r="P9" s="55"/>
+      <c r="Q9" s="55"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="56"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="49" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="32" t="s">
+      <c r="E12" s="58"/>
+      <c r="F12" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="26" t="s">
+      <c r="G12" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="32" t="s">
+      <c r="H12" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="28" t="s">
+      <c r="I12" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="29"/>
-      <c r="K12" s="34" t="s">
+      <c r="J12" s="58"/>
+      <c r="K12" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="L12" s="35"/>
-      <c r="M12" s="26" t="s">
+      <c r="L12" s="46"/>
+      <c r="M12" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="N12" s="26" t="s">
+      <c r="N12" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="O12" s="34" t="s">
+      <c r="O12" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="P12" s="35"/>
+      <c r="P12" s="46"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
+      <c r="A13" s="50"/>
       <c r="B13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="37"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="36"/>
-      <c r="P13" s="37"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="60"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="50"/>
+      <c r="O13" s="47"/>
+      <c r="P13" s="48"/>
     </row>
     <row r="14" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="38">
+      <c r="C14" s="20">
         <v>30000012346</v>
       </c>
-      <c r="D14" s="44" t="s">
+      <c r="D14" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="45"/>
-      <c r="F14" s="46" t="s">
+      <c r="E14" s="41"/>
+      <c r="F14" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="38">
+      <c r="G14" s="20">
         <v>1324567</v>
       </c>
-      <c r="H14" s="41" t="s">
+      <c r="H14" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="I14" s="51"/>
-      <c r="J14" s="52"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="32"/>
       <c r="K14" s="10" t="s">
         <v>1</v>
       </c>
@@ -1227,18 +1261,18 @@
       <c r="P14" s="11"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="39"/>
-      <c r="B15" s="42"/>
-      <c r="C15" s="39"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="21"/>
       <c r="D15" s="16" t="s">
         <v>1</v>
       </c>
       <c r="E15" s="17"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="54"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="34"/>
       <c r="K15" s="12"/>
       <c r="L15" s="13"/>
       <c r="M15" s="8"/>
@@ -1247,18 +1281,18 @@
       <c r="P15" s="13"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
-      <c r="B16" s="43"/>
-      <c r="C16" s="40"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="22"/>
       <c r="D16" s="18" t="s">
         <v>1</v>
       </c>
       <c r="E16" s="19"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="43"/>
-      <c r="I16" s="55"/>
-      <c r="J16" s="56"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="36"/>
       <c r="K16" s="14"/>
       <c r="L16" s="15"/>
       <c r="M16" s="9"/>
@@ -1267,30 +1301,30 @@
       <c r="P16" s="15"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="38">
+      <c r="A17" s="20">
         <v>2</v>
       </c>
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="38">
+      <c r="C17" s="20">
         <v>30000062842</v>
       </c>
-      <c r="D17" s="44" t="s">
+      <c r="D17" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="49"/>
-      <c r="F17" s="50" t="s">
+      <c r="E17" s="40"/>
+      <c r="F17" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="38">
+      <c r="G17" s="20">
         <v>3108437301</v>
       </c>
-      <c r="H17" s="41" t="s">
+      <c r="H17" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="I17" s="51"/>
-      <c r="J17" s="52"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="32"/>
       <c r="K17" s="10"/>
       <c r="L17" s="11"/>
       <c r="M17" s="7"/>
@@ -1299,16 +1333,16 @@
       <c r="P17" s="11"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="39"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="39"/>
+      <c r="A18" s="21"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="21"/>
       <c r="D18" s="16"/>
       <c r="E18" s="17"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="54"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="34"/>
       <c r="K18" s="12"/>
       <c r="L18" s="13"/>
       <c r="M18" s="8"/>
@@ -1317,16 +1351,16 @@
       <c r="P18" s="13"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="40"/>
-      <c r="B19" s="43"/>
-      <c r="C19" s="40"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="22"/>
       <c r="D19" s="18"/>
       <c r="E19" s="19"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="55"/>
-      <c r="J19" s="56"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="36"/>
       <c r="K19" s="14"/>
       <c r="L19" s="15"/>
       <c r="M19" s="9"/>
@@ -1335,30 +1369,30 @@
       <c r="P19" s="15"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="38">
+      <c r="A20" s="20">
         <v>3</v>
       </c>
-      <c r="B20" s="41" t="s">
+      <c r="B20" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="38">
+      <c r="C20" s="20">
         <v>30000070034</v>
       </c>
-      <c r="D20" s="44" t="s">
+      <c r="D20" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="49"/>
-      <c r="F20" s="50" t="s">
+      <c r="E20" s="40"/>
+      <c r="F20" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="38">
+      <c r="G20" s="20">
         <v>3189128918</v>
       </c>
-      <c r="H20" s="41" t="s">
+      <c r="H20" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="I20" s="51"/>
-      <c r="J20" s="52"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="32"/>
       <c r="K20" s="10"/>
       <c r="L20" s="11"/>
       <c r="M20" s="7"/>
@@ -1367,16 +1401,16 @@
       <c r="P20" s="11"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="39"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="39"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="21"/>
       <c r="D21" s="16"/>
       <c r="E21" s="17"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="53"/>
-      <c r="J21" s="54"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="34"/>
       <c r="K21" s="12"/>
       <c r="L21" s="13"/>
       <c r="M21" s="8"/>
@@ -1385,16 +1419,16 @@
       <c r="P21" s="13"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="40"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="40"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="22"/>
       <c r="D22" s="18"/>
       <c r="E22" s="19"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="55"/>
-      <c r="J22" s="56"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="36"/>
       <c r="K22" s="14"/>
       <c r="L22" s="15"/>
       <c r="M22" s="9"/>
@@ -1403,30 +1437,30 @@
       <c r="P22" s="15"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="38">
+      <c r="A23" s="20">
         <v>4</v>
       </c>
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="38">
+      <c r="C23" s="20">
         <v>30000070035</v>
       </c>
-      <c r="D23" s="44" t="s">
+      <c r="D23" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="49"/>
-      <c r="F23" s="50" t="s">
+      <c r="E23" s="40"/>
+      <c r="F23" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="G23" s="38">
+      <c r="G23" s="20">
         <v>3189128918</v>
       </c>
-      <c r="H23" s="41" t="s">
+      <c r="H23" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="I23" s="51"/>
-      <c r="J23" s="52"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="32"/>
       <c r="K23" s="10"/>
       <c r="L23" s="11"/>
       <c r="M23" s="7"/>
@@ -1435,16 +1469,16 @@
       <c r="P23" s="11"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="39"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="39"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="21"/>
       <c r="D24" s="16"/>
       <c r="E24" s="17"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="53"/>
-      <c r="J24" s="54"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="34"/>
       <c r="K24" s="12"/>
       <c r="L24" s="13"/>
       <c r="M24" s="8"/>
@@ -1453,16 +1487,16 @@
       <c r="P24" s="13"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="40"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="40"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="22"/>
       <c r="D25" s="18"/>
       <c r="E25" s="19"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="55"/>
-      <c r="J25" s="56"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="35"/>
+      <c r="J25" s="36"/>
       <c r="K25" s="14"/>
       <c r="L25" s="15"/>
       <c r="M25" s="9"/>
@@ -1471,30 +1505,30 @@
       <c r="P25" s="15"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="38">
+      <c r="A26" s="20">
         <v>5</v>
       </c>
-      <c r="B26" s="41" t="s">
+      <c r="B26" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="38">
+      <c r="C26" s="20">
         <v>30000070036</v>
       </c>
-      <c r="D26" s="44" t="s">
+      <c r="D26" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E26" s="49"/>
-      <c r="F26" s="50" t="s">
+      <c r="E26" s="40"/>
+      <c r="F26" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="G26" s="38">
+      <c r="G26" s="20">
         <v>3189128918</v>
       </c>
-      <c r="H26" s="41" t="s">
+      <c r="H26" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="I26" s="51"/>
-      <c r="J26" s="52"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="32"/>
       <c r="K26" s="10"/>
       <c r="L26" s="11"/>
       <c r="M26" s="7"/>
@@ -1503,16 +1537,16 @@
       <c r="P26" s="11"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="39"/>
-      <c r="B27" s="42"/>
-      <c r="C27" s="39"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="21"/>
       <c r="D27" s="16"/>
       <c r="E27" s="17"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="53"/>
-      <c r="J27" s="54"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="34"/>
       <c r="K27" s="12"/>
       <c r="L27" s="13"/>
       <c r="M27" s="8"/>
@@ -1521,16 +1555,16 @@
       <c r="P27" s="13"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="40"/>
-      <c r="B28" s="43"/>
-      <c r="C28" s="40"/>
+      <c r="A28" s="22"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="22"/>
       <c r="D28" s="18"/>
       <c r="E28" s="19"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="40"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="55"/>
-      <c r="J28" s="56"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="36"/>
       <c r="K28" s="14"/>
       <c r="L28" s="15"/>
       <c r="M28" s="9"/>
@@ -1539,30 +1573,30 @@
       <c r="P28" s="15"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="38">
+      <c r="A29" s="20">
         <v>6</v>
       </c>
-      <c r="B29" s="41" t="s">
+      <c r="B29" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="38">
+      <c r="C29" s="20">
         <v>30000070037</v>
       </c>
-      <c r="D29" s="44" t="s">
+      <c r="D29" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="49"/>
-      <c r="F29" s="50" t="s">
+      <c r="E29" s="40"/>
+      <c r="F29" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="G29" s="38">
+      <c r="G29" s="20">
         <v>3189128918</v>
       </c>
-      <c r="H29" s="41" t="s">
+      <c r="H29" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="I29" s="51"/>
-      <c r="J29" s="52"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="32"/>
       <c r="K29" s="10"/>
       <c r="L29" s="11"/>
       <c r="M29" s="7"/>
@@ -1571,16 +1605,16 @@
       <c r="P29" s="11"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="39"/>
-      <c r="B30" s="42"/>
-      <c r="C30" s="39"/>
+      <c r="A30" s="21"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="21"/>
       <c r="D30" s="16"/>
       <c r="E30" s="17"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="53"/>
-      <c r="J30" s="54"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="34"/>
       <c r="K30" s="12"/>
       <c r="L30" s="13"/>
       <c r="M30" s="8"/>
@@ -1589,16 +1623,16 @@
       <c r="P30" s="13"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" s="40"/>
-      <c r="B31" s="43"/>
-      <c r="C31" s="40"/>
+      <c r="A31" s="22"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="22"/>
       <c r="D31" s="18"/>
       <c r="E31" s="19"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="43"/>
-      <c r="I31" s="55"/>
-      <c r="J31" s="56"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="35"/>
+      <c r="J31" s="36"/>
       <c r="K31" s="14"/>
       <c r="L31" s="15"/>
       <c r="M31" s="9"/>
@@ -1607,30 +1641,30 @@
       <c r="P31" s="15"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="38">
+      <c r="A32" s="20">
         <v>7</v>
       </c>
-      <c r="B32" s="41" t="s">
+      <c r="B32" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="38">
+      <c r="C32" s="20">
         <v>30000070038</v>
       </c>
-      <c r="D32" s="44" t="s">
+      <c r="D32" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E32" s="49"/>
-      <c r="F32" s="50" t="s">
+      <c r="E32" s="40"/>
+      <c r="F32" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="G32" s="38">
+      <c r="G32" s="20">
         <v>3189128918</v>
       </c>
-      <c r="H32" s="41" t="s">
+      <c r="H32" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="I32" s="51"/>
-      <c r="J32" s="52"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="32"/>
       <c r="K32" s="10"/>
       <c r="L32" s="11"/>
       <c r="M32" s="7"/>
@@ -1639,16 +1673,16 @@
       <c r="P32" s="11"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="39"/>
-      <c r="B33" s="42"/>
-      <c r="C33" s="39"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="21"/>
       <c r="D33" s="16"/>
       <c r="E33" s="17"/>
-      <c r="F33" s="42"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="42"/>
-      <c r="I33" s="53"/>
-      <c r="J33" s="54"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="34"/>
       <c r="K33" s="12"/>
       <c r="L33" s="13"/>
       <c r="M33" s="8"/>
@@ -1657,16 +1691,16 @@
       <c r="P33" s="13"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="40"/>
-      <c r="B34" s="43"/>
-      <c r="C34" s="40"/>
+      <c r="A34" s="22"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="22"/>
       <c r="D34" s="18"/>
       <c r="E34" s="19"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="43"/>
-      <c r="I34" s="55"/>
-      <c r="J34" s="56"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="36"/>
       <c r="K34" s="14"/>
       <c r="L34" s="15"/>
       <c r="M34" s="9"/>
@@ -1675,30 +1709,30 @@
       <c r="P34" s="15"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="38">
+      <c r="A35" s="20">
         <v>8</v>
       </c>
-      <c r="B35" s="41" t="s">
+      <c r="B35" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C35" s="38">
+      <c r="C35" s="20">
         <v>30000070039</v>
       </c>
-      <c r="D35" s="44" t="s">
+      <c r="D35" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E35" s="49"/>
-      <c r="F35" s="50" t="s">
+      <c r="E35" s="40"/>
+      <c r="F35" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="G35" s="38">
+      <c r="G35" s="20">
         <v>3189128918</v>
       </c>
-      <c r="H35" s="41" t="s">
+      <c r="H35" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="I35" s="51"/>
-      <c r="J35" s="52"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="32"/>
       <c r="K35" s="10"/>
       <c r="L35" s="11"/>
       <c r="M35" s="7"/>
@@ -1707,16 +1741,16 @@
       <c r="P35" s="11"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A36" s="39"/>
-      <c r="B36" s="42"/>
-      <c r="C36" s="39"/>
+      <c r="A36" s="21"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="21"/>
       <c r="D36" s="16"/>
       <c r="E36" s="17"/>
-      <c r="F36" s="42"/>
-      <c r="G36" s="39"/>
-      <c r="H36" s="42"/>
-      <c r="I36" s="53"/>
-      <c r="J36" s="54"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="34"/>
       <c r="K36" s="12"/>
       <c r="L36" s="13"/>
       <c r="M36" s="8"/>
@@ -1725,16 +1759,16 @@
       <c r="P36" s="13"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A37" s="40"/>
-      <c r="B37" s="43"/>
-      <c r="C37" s="40"/>
+      <c r="A37" s="22"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="22"/>
       <c r="D37" s="18"/>
       <c r="E37" s="19"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="40"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="55"/>
-      <c r="J37" s="56"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="36"/>
       <c r="K37" s="14"/>
       <c r="L37" s="15"/>
       <c r="M37" s="9"/>
@@ -1743,30 +1777,30 @@
       <c r="P37" s="15"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A38" s="38">
+      <c r="A38" s="20">
         <v>9</v>
       </c>
-      <c r="B38" s="41" t="s">
+      <c r="B38" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C38" s="38">
+      <c r="C38" s="20">
         <v>30000070040</v>
       </c>
-      <c r="D38" s="44" t="s">
+      <c r="D38" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E38" s="49"/>
-      <c r="F38" s="50" t="s">
+      <c r="E38" s="40"/>
+      <c r="F38" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="G38" s="38">
+      <c r="G38" s="20">
         <v>3189128918</v>
       </c>
-      <c r="H38" s="41" t="s">
+      <c r="H38" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="I38" s="51"/>
-      <c r="J38" s="52"/>
+      <c r="I38" s="31"/>
+      <c r="J38" s="32"/>
       <c r="K38" s="10"/>
       <c r="L38" s="11"/>
       <c r="M38" s="7"/>
@@ -1775,16 +1809,16 @@
       <c r="P38" s="11"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39" s="39"/>
-      <c r="B39" s="42"/>
-      <c r="C39" s="39"/>
+      <c r="A39" s="21"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="21"/>
       <c r="D39" s="16"/>
       <c r="E39" s="17"/>
-      <c r="F39" s="42"/>
-      <c r="G39" s="39"/>
-      <c r="H39" s="42"/>
-      <c r="I39" s="53"/>
-      <c r="J39" s="54"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="34"/>
       <c r="K39" s="12"/>
       <c r="L39" s="13"/>
       <c r="M39" s="8"/>
@@ -1793,16 +1827,16 @@
       <c r="P39" s="13"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A40" s="40"/>
-      <c r="B40" s="43"/>
-      <c r="C40" s="40"/>
+      <c r="A40" s="22"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="22"/>
       <c r="D40" s="18"/>
       <c r="E40" s="19"/>
-      <c r="F40" s="43"/>
-      <c r="G40" s="40"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="55"/>
-      <c r="J40" s="56"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="35"/>
+      <c r="J40" s="36"/>
       <c r="K40" s="14"/>
       <c r="L40" s="15"/>
       <c r="M40" s="9"/>
@@ -1811,30 +1845,30 @@
       <c r="P40" s="15"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A41" s="38">
+      <c r="A41" s="20">
         <v>10</v>
       </c>
-      <c r="B41" s="41" t="s">
+      <c r="B41" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C41" s="38">
+      <c r="C41" s="20">
         <v>30000070041</v>
       </c>
-      <c r="D41" s="44" t="s">
+      <c r="D41" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E41" s="49"/>
-      <c r="F41" s="50" t="s">
+      <c r="E41" s="40"/>
+      <c r="F41" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="G41" s="38">
+      <c r="G41" s="20">
         <v>3189128918</v>
       </c>
-      <c r="H41" s="41" t="s">
+      <c r="H41" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="I41" s="51"/>
-      <c r="J41" s="52"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="32"/>
       <c r="K41" s="10"/>
       <c r="L41" s="11"/>
       <c r="M41" s="7"/>
@@ -1843,16 +1877,16 @@
       <c r="P41" s="11"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A42" s="39"/>
-      <c r="B42" s="42"/>
-      <c r="C42" s="39"/>
+      <c r="A42" s="21"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="21"/>
       <c r="D42" s="16"/>
       <c r="E42" s="17"/>
-      <c r="F42" s="42"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="42"/>
-      <c r="I42" s="53"/>
-      <c r="J42" s="54"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="33"/>
+      <c r="J42" s="34"/>
       <c r="K42" s="12"/>
       <c r="L42" s="13"/>
       <c r="M42" s="8"/>
@@ -1861,16 +1895,16 @@
       <c r="P42" s="13"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43" s="40"/>
-      <c r="B43" s="43"/>
-      <c r="C43" s="40"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="22"/>
       <c r="D43" s="18"/>
       <c r="E43" s="19"/>
-      <c r="F43" s="43"/>
-      <c r="G43" s="40"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="55"/>
-      <c r="J43" s="56"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="25"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="36"/>
       <c r="K43" s="14"/>
       <c r="L43" s="15"/>
       <c r="M43" s="9"/>
@@ -1879,30 +1913,30 @@
       <c r="P43" s="15"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A44" s="38">
+      <c r="A44" s="20">
         <v>11</v>
       </c>
-      <c r="B44" s="41" t="s">
+      <c r="B44" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C44" s="38">
+      <c r="C44" s="20">
         <v>30000070042</v>
       </c>
-      <c r="D44" s="44" t="s">
+      <c r="D44" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E44" s="49"/>
-      <c r="F44" s="50" t="s">
+      <c r="E44" s="40"/>
+      <c r="F44" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="G44" s="38">
+      <c r="G44" s="20">
         <v>3189128918</v>
       </c>
-      <c r="H44" s="41" t="s">
+      <c r="H44" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="I44" s="51"/>
-      <c r="J44" s="52"/>
+      <c r="I44" s="31"/>
+      <c r="J44" s="32"/>
       <c r="K44" s="10"/>
       <c r="L44" s="11"/>
       <c r="M44" s="7"/>
@@ -1911,16 +1945,16 @@
       <c r="P44" s="11"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" s="39"/>
-      <c r="B45" s="42"/>
-      <c r="C45" s="39"/>
+      <c r="A45" s="21"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="21"/>
       <c r="D45" s="16"/>
       <c r="E45" s="17"/>
-      <c r="F45" s="42"/>
-      <c r="G45" s="39"/>
-      <c r="H45" s="42"/>
-      <c r="I45" s="53"/>
-      <c r="J45" s="54"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="33"/>
+      <c r="J45" s="34"/>
       <c r="K45" s="12"/>
       <c r="L45" s="13"/>
       <c r="M45" s="8"/>
@@ -1929,16 +1963,16 @@
       <c r="P45" s="13"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46" s="40"/>
-      <c r="B46" s="43"/>
-      <c r="C46" s="40"/>
+      <c r="A46" s="22"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="22"/>
       <c r="D46" s="18"/>
       <c r="E46" s="19"/>
-      <c r="F46" s="43"/>
-      <c r="G46" s="40"/>
-      <c r="H46" s="43"/>
-      <c r="I46" s="55"/>
-      <c r="J46" s="56"/>
+      <c r="F46" s="25"/>
+      <c r="G46" s="22"/>
+      <c r="H46" s="25"/>
+      <c r="I46" s="35"/>
+      <c r="J46" s="36"/>
       <c r="K46" s="14"/>
       <c r="L46" s="15"/>
       <c r="M46" s="9"/>
@@ -1947,30 +1981,30 @@
       <c r="P46" s="15"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A47" s="38">
+      <c r="A47" s="20">
         <v>12</v>
       </c>
-      <c r="B47" s="41" t="s">
+      <c r="B47" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C47" s="38">
+      <c r="C47" s="20">
         <v>30000070043</v>
       </c>
-      <c r="D47" s="44" t="s">
+      <c r="D47" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E47" s="49"/>
-      <c r="F47" s="50" t="s">
+      <c r="E47" s="40"/>
+      <c r="F47" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="G47" s="38">
+      <c r="G47" s="20">
         <v>3189128918</v>
       </c>
-      <c r="H47" s="41" t="s">
+      <c r="H47" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="I47" s="51"/>
-      <c r="J47" s="52"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="32"/>
       <c r="K47" s="10"/>
       <c r="L47" s="11"/>
       <c r="M47" s="7"/>
@@ -1979,16 +2013,16 @@
       <c r="P47" s="11"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A48" s="39"/>
-      <c r="B48" s="42"/>
-      <c r="C48" s="39"/>
+      <c r="A48" s="21"/>
+      <c r="B48" s="24"/>
+      <c r="C48" s="21"/>
       <c r="D48" s="16"/>
       <c r="E48" s="17"/>
-      <c r="F48" s="42"/>
-      <c r="G48" s="39"/>
-      <c r="H48" s="42"/>
-      <c r="I48" s="53"/>
-      <c r="J48" s="54"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="21"/>
+      <c r="H48" s="24"/>
+      <c r="I48" s="33"/>
+      <c r="J48" s="34"/>
       <c r="K48" s="12"/>
       <c r="L48" s="13"/>
       <c r="M48" s="8"/>
@@ -1997,16 +2031,16 @@
       <c r="P48" s="13"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A49" s="40"/>
-      <c r="B49" s="43"/>
-      <c r="C49" s="40"/>
+      <c r="A49" s="22"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="22"/>
       <c r="D49" s="18"/>
       <c r="E49" s="19"/>
-      <c r="F49" s="43"/>
-      <c r="G49" s="40"/>
-      <c r="H49" s="43"/>
-      <c r="I49" s="55"/>
-      <c r="J49" s="56"/>
+      <c r="F49" s="25"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="25"/>
+      <c r="I49" s="35"/>
+      <c r="J49" s="36"/>
       <c r="K49" s="14"/>
       <c r="L49" s="15"/>
       <c r="M49" s="9"/>
@@ -2015,30 +2049,30 @@
       <c r="P49" s="15"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A50" s="38">
+      <c r="A50" s="20">
         <v>13</v>
       </c>
-      <c r="B50" s="41" t="s">
+      <c r="B50" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C50" s="38">
+      <c r="C50" s="20">
         <v>30000070044</v>
       </c>
-      <c r="D50" s="44" t="s">
+      <c r="D50" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E50" s="49"/>
-      <c r="F50" s="50" t="s">
+      <c r="E50" s="40"/>
+      <c r="F50" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="G50" s="38">
+      <c r="G50" s="20">
         <v>3189128918</v>
       </c>
-      <c r="H50" s="41" t="s">
+      <c r="H50" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="I50" s="51"/>
-      <c r="J50" s="52"/>
+      <c r="I50" s="31"/>
+      <c r="J50" s="32"/>
       <c r="K50" s="10"/>
       <c r="L50" s="11"/>
       <c r="M50" s="7"/>
@@ -2047,16 +2081,16 @@
       <c r="P50" s="11"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A51" s="39"/>
-      <c r="B51" s="42"/>
-      <c r="C51" s="39"/>
+      <c r="A51" s="21"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="21"/>
       <c r="D51" s="16"/>
       <c r="E51" s="17"/>
-      <c r="F51" s="42"/>
-      <c r="G51" s="39"/>
-      <c r="H51" s="42"/>
-      <c r="I51" s="53"/>
-      <c r="J51" s="54"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="21"/>
+      <c r="H51" s="24"/>
+      <c r="I51" s="33"/>
+      <c r="J51" s="34"/>
       <c r="K51" s="12"/>
       <c r="L51" s="13"/>
       <c r="M51" s="8"/>
@@ -2065,16 +2099,16 @@
       <c r="P51" s="13"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A52" s="40"/>
-      <c r="B52" s="43"/>
-      <c r="C52" s="40"/>
+      <c r="A52" s="22"/>
+      <c r="B52" s="25"/>
+      <c r="C52" s="22"/>
       <c r="D52" s="18"/>
       <c r="E52" s="19"/>
-      <c r="F52" s="43"/>
-      <c r="G52" s="40"/>
-      <c r="H52" s="43"/>
-      <c r="I52" s="55"/>
-      <c r="J52" s="56"/>
+      <c r="F52" s="25"/>
+      <c r="G52" s="22"/>
+      <c r="H52" s="25"/>
+      <c r="I52" s="35"/>
+      <c r="J52" s="36"/>
       <c r="K52" s="14"/>
       <c r="L52" s="15"/>
       <c r="M52" s="9"/>
@@ -2083,30 +2117,30 @@
       <c r="P52" s="15"/>
     </row>
     <row r="53" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="38">
+      <c r="A53" s="20">
         <v>14</v>
       </c>
-      <c r="B53" s="41" t="s">
+      <c r="B53" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="38">
+      <c r="C53" s="20">
         <v>30000070045</v>
       </c>
-      <c r="D53" s="44" t="s">
+      <c r="D53" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E53" s="62"/>
-      <c r="F53" s="50" t="s">
+      <c r="E53" s="27"/>
+      <c r="F53" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="G53" s="38">
+      <c r="G53" s="20">
         <v>3189128918</v>
       </c>
-      <c r="H53" s="41" t="s">
+      <c r="H53" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="I53" s="51"/>
-      <c r="J53" s="52"/>
+      <c r="I53" s="31"/>
+      <c r="J53" s="32"/>
       <c r="K53" s="10"/>
       <c r="L53" s="11"/>
       <c r="M53" s="7"/>
@@ -2115,16 +2149,16 @@
       <c r="P53" s="11"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A54" s="39"/>
-      <c r="B54" s="42"/>
-      <c r="C54" s="39"/>
+      <c r="A54" s="21"/>
+      <c r="B54" s="24"/>
+      <c r="C54" s="21"/>
       <c r="D54" s="16"/>
       <c r="E54" s="17"/>
-      <c r="F54" s="60"/>
-      <c r="G54" s="39"/>
-      <c r="H54" s="42"/>
-      <c r="I54" s="53"/>
-      <c r="J54" s="54"/>
+      <c r="F54" s="29"/>
+      <c r="G54" s="21"/>
+      <c r="H54" s="24"/>
+      <c r="I54" s="33"/>
+      <c r="J54" s="34"/>
       <c r="K54" s="12"/>
       <c r="L54" s="13"/>
       <c r="M54" s="8"/>
@@ -2133,16 +2167,16 @@
       <c r="P54" s="13"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A55" s="40"/>
-      <c r="B55" s="43"/>
-      <c r="C55" s="40"/>
+      <c r="A55" s="22"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="22"/>
       <c r="D55" s="18"/>
       <c r="E55" s="19"/>
-      <c r="F55" s="61"/>
-      <c r="G55" s="40"/>
-      <c r="H55" s="43"/>
-      <c r="I55" s="55"/>
-      <c r="J55" s="56"/>
+      <c r="F55" s="30"/>
+      <c r="G55" s="22"/>
+      <c r="H55" s="25"/>
+      <c r="I55" s="35"/>
+      <c r="J55" s="36"/>
       <c r="K55" s="14"/>
       <c r="L55" s="15"/>
       <c r="M55" s="9"/>
@@ -2151,30 +2185,30 @@
       <c r="P55" s="15"/>
     </row>
     <row r="56" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="38">
+      <c r="A56" s="20">
         <v>15</v>
       </c>
-      <c r="B56" s="41" t="s">
+      <c r="B56" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C56" s="38">
+      <c r="C56" s="20">
         <v>30000070046</v>
       </c>
-      <c r="D56" s="44" t="s">
+      <c r="D56" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E56" s="62"/>
-      <c r="F56" s="50" t="s">
+      <c r="E56" s="27"/>
+      <c r="F56" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="G56" s="38">
+      <c r="G56" s="20">
         <v>3189128918</v>
       </c>
-      <c r="H56" s="41" t="s">
+      <c r="H56" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="I56" s="51"/>
-      <c r="J56" s="52"/>
+      <c r="I56" s="31"/>
+      <c r="J56" s="32"/>
       <c r="K56" s="10"/>
       <c r="L56" s="11"/>
       <c r="M56" s="7"/>
@@ -2183,16 +2217,16 @@
       <c r="P56" s="11"/>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A57" s="39"/>
-      <c r="B57" s="42"/>
-      <c r="C57" s="39"/>
+      <c r="A57" s="21"/>
+      <c r="B57" s="24"/>
+      <c r="C57" s="21"/>
       <c r="D57" s="16"/>
       <c r="E57" s="17"/>
-      <c r="F57" s="60"/>
-      <c r="G57" s="39"/>
-      <c r="H57" s="42"/>
-      <c r="I57" s="53"/>
-      <c r="J57" s="54"/>
+      <c r="F57" s="29"/>
+      <c r="G57" s="21"/>
+      <c r="H57" s="24"/>
+      <c r="I57" s="33"/>
+      <c r="J57" s="34"/>
       <c r="K57" s="12"/>
       <c r="L57" s="13"/>
       <c r="M57" s="8"/>
@@ -2201,16 +2235,16 @@
       <c r="P57" s="13"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A58" s="40"/>
-      <c r="B58" s="43"/>
-      <c r="C58" s="40"/>
+      <c r="A58" s="22"/>
+      <c r="B58" s="25"/>
+      <c r="C58" s="22"/>
       <c r="D58" s="18"/>
       <c r="E58" s="19"/>
-      <c r="F58" s="61"/>
-      <c r="G58" s="40"/>
-      <c r="H58" s="43"/>
-      <c r="I58" s="55"/>
-      <c r="J58" s="56"/>
+      <c r="F58" s="30"/>
+      <c r="G58" s="22"/>
+      <c r="H58" s="25"/>
+      <c r="I58" s="35"/>
+      <c r="J58" s="36"/>
       <c r="K58" s="14"/>
       <c r="L58" s="15"/>
       <c r="M58" s="9"/>
@@ -2219,30 +2253,30 @@
       <c r="P58" s="15"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A59" s="38">
+      <c r="A59" s="20">
         <v>16</v>
       </c>
-      <c r="B59" s="41" t="s">
+      <c r="B59" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C59" s="38">
+      <c r="C59" s="20">
         <v>30000070047</v>
       </c>
-      <c r="D59" s="44" t="s">
+      <c r="D59" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E59" s="62"/>
-      <c r="F59" s="50" t="s">
+      <c r="E59" s="27"/>
+      <c r="F59" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="G59" s="38">
+      <c r="G59" s="20">
         <v>3189128918</v>
       </c>
-      <c r="H59" s="41" t="s">
+      <c r="H59" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="I59" s="51"/>
-      <c r="J59" s="52"/>
+      <c r="I59" s="31"/>
+      <c r="J59" s="32"/>
       <c r="K59" s="10"/>
       <c r="L59" s="11"/>
       <c r="M59" s="7"/>
@@ -2251,16 +2285,16 @@
       <c r="P59" s="11"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A60" s="39"/>
-      <c r="B60" s="42"/>
-      <c r="C60" s="39"/>
+      <c r="A60" s="21"/>
+      <c r="B60" s="24"/>
+      <c r="C60" s="21"/>
       <c r="D60" s="16"/>
       <c r="E60" s="17"/>
-      <c r="F60" s="60"/>
-      <c r="G60" s="39"/>
-      <c r="H60" s="42"/>
-      <c r="I60" s="53"/>
-      <c r="J60" s="54"/>
+      <c r="F60" s="29"/>
+      <c r="G60" s="21"/>
+      <c r="H60" s="24"/>
+      <c r="I60" s="33"/>
+      <c r="J60" s="34"/>
       <c r="K60" s="12"/>
       <c r="L60" s="13"/>
       <c r="M60" s="8"/>
@@ -2269,16 +2303,16 @@
       <c r="P60" s="13"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A61" s="40"/>
-      <c r="B61" s="43"/>
-      <c r="C61" s="40"/>
+      <c r="A61" s="22"/>
+      <c r="B61" s="25"/>
+      <c r="C61" s="22"/>
       <c r="D61" s="18"/>
       <c r="E61" s="19"/>
-      <c r="F61" s="61"/>
-      <c r="G61" s="40"/>
-      <c r="H61" s="43"/>
-      <c r="I61" s="55"/>
-      <c r="J61" s="56"/>
+      <c r="F61" s="30"/>
+      <c r="G61" s="22"/>
+      <c r="H61" s="25"/>
+      <c r="I61" s="35"/>
+      <c r="J61" s="36"/>
       <c r="K61" s="14"/>
       <c r="L61" s="15"/>
       <c r="M61" s="9"/>
@@ -2287,30 +2321,30 @@
       <c r="P61" s="15"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A62" s="38">
+      <c r="A62" s="20">
         <v>17</v>
       </c>
-      <c r="B62" s="41" t="s">
+      <c r="B62" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C62" s="38">
+      <c r="C62" s="20">
         <v>30000070048</v>
       </c>
-      <c r="D62" s="44" t="s">
+      <c r="D62" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E62" s="62"/>
-      <c r="F62" s="50" t="s">
+      <c r="E62" s="27"/>
+      <c r="F62" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="G62" s="38">
+      <c r="G62" s="20">
         <v>3189128918</v>
       </c>
-      <c r="H62" s="41" t="s">
+      <c r="H62" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="I62" s="51"/>
-      <c r="J62" s="52"/>
+      <c r="I62" s="31"/>
+      <c r="J62" s="32"/>
       <c r="K62" s="10"/>
       <c r="L62" s="11"/>
       <c r="M62" s="7"/>
@@ -2319,16 +2353,16 @@
       <c r="P62" s="11"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A63" s="39"/>
-      <c r="B63" s="42"/>
-      <c r="C63" s="39"/>
+      <c r="A63" s="21"/>
+      <c r="B63" s="24"/>
+      <c r="C63" s="21"/>
       <c r="D63" s="16"/>
       <c r="E63" s="17"/>
-      <c r="F63" s="60"/>
-      <c r="G63" s="39"/>
-      <c r="H63" s="42"/>
-      <c r="I63" s="53"/>
-      <c r="J63" s="54"/>
+      <c r="F63" s="29"/>
+      <c r="G63" s="21"/>
+      <c r="H63" s="24"/>
+      <c r="I63" s="33"/>
+      <c r="J63" s="34"/>
       <c r="K63" s="12"/>
       <c r="L63" s="13"/>
       <c r="M63" s="8"/>
@@ -2337,16 +2371,16 @@
       <c r="P63" s="13"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A64" s="40"/>
-      <c r="B64" s="43"/>
-      <c r="C64" s="40"/>
+      <c r="A64" s="22"/>
+      <c r="B64" s="25"/>
+      <c r="C64" s="22"/>
       <c r="D64" s="18"/>
       <c r="E64" s="19"/>
-      <c r="F64" s="61"/>
-      <c r="G64" s="40"/>
-      <c r="H64" s="43"/>
-      <c r="I64" s="55"/>
-      <c r="J64" s="56"/>
+      <c r="F64" s="30"/>
+      <c r="G64" s="22"/>
+      <c r="H64" s="25"/>
+      <c r="I64" s="35"/>
+      <c r="J64" s="36"/>
       <c r="K64" s="14"/>
       <c r="L64" s="15"/>
       <c r="M64" s="9"/>
@@ -2355,30 +2389,30 @@
       <c r="P64" s="15"/>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A65" s="38">
+      <c r="A65" s="20">
         <v>18</v>
       </c>
-      <c r="B65" s="41" t="s">
+      <c r="B65" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C65" s="38">
+      <c r="C65" s="20">
         <v>30000070049</v>
       </c>
-      <c r="D65" s="44" t="s">
+      <c r="D65" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E65" s="62"/>
-      <c r="F65" s="50" t="s">
+      <c r="E65" s="27"/>
+      <c r="F65" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="G65" s="38">
+      <c r="G65" s="20">
         <v>3189128918</v>
       </c>
-      <c r="H65" s="41" t="s">
+      <c r="H65" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="I65" s="51"/>
-      <c r="J65" s="52"/>
+      <c r="I65" s="31"/>
+      <c r="J65" s="32"/>
       <c r="K65" s="10"/>
       <c r="L65" s="11"/>
       <c r="M65" s="7"/>
@@ -2387,16 +2421,16 @@
       <c r="P65" s="11"/>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A66" s="39"/>
-      <c r="B66" s="42"/>
-      <c r="C66" s="39"/>
+      <c r="A66" s="21"/>
+      <c r="B66" s="24"/>
+      <c r="C66" s="21"/>
       <c r="D66" s="16"/>
       <c r="E66" s="17"/>
-      <c r="F66" s="60"/>
-      <c r="G66" s="39"/>
-      <c r="H66" s="42"/>
-      <c r="I66" s="53"/>
-      <c r="J66" s="54"/>
+      <c r="F66" s="29"/>
+      <c r="G66" s="21"/>
+      <c r="H66" s="24"/>
+      <c r="I66" s="33"/>
+      <c r="J66" s="34"/>
       <c r="K66" s="12"/>
       <c r="L66" s="13"/>
       <c r="M66" s="8"/>
@@ -2405,16 +2439,16 @@
       <c r="P66" s="13"/>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A67" s="40"/>
-      <c r="B67" s="43"/>
-      <c r="C67" s="40"/>
+      <c r="A67" s="22"/>
+      <c r="B67" s="25"/>
+      <c r="C67" s="22"/>
       <c r="D67" s="18"/>
       <c r="E67" s="19"/>
-      <c r="F67" s="61"/>
-      <c r="G67" s="40"/>
-      <c r="H67" s="43"/>
-      <c r="I67" s="55"/>
-      <c r="J67" s="56"/>
+      <c r="F67" s="30"/>
+      <c r="G67" s="22"/>
+      <c r="H67" s="25"/>
+      <c r="I67" s="35"/>
+      <c r="J67" s="36"/>
       <c r="K67" s="14"/>
       <c r="L67" s="15"/>
       <c r="M67" s="9"/>
@@ -2423,65 +2457,65 @@
       <c r="P67" s="15"/>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A68" s="57"/>
-      <c r="B68" s="57"/>
-      <c r="C68" s="57"/>
-      <c r="D68" s="57"/>
-      <c r="E68" s="57"/>
-      <c r="F68" s="57"/>
-      <c r="G68" s="57"/>
-      <c r="H68" s="57"/>
-      <c r="I68" s="57"/>
-      <c r="J68" s="57"/>
-      <c r="K68" s="57"/>
-      <c r="L68" s="57"/>
-      <c r="M68" s="57"/>
-      <c r="N68" s="57"/>
-      <c r="O68" s="57"/>
-      <c r="P68" s="57"/>
-      <c r="Q68" s="57"/>
+      <c r="A68" s="37"/>
+      <c r="B68" s="37"/>
+      <c r="C68" s="37"/>
+      <c r="D68" s="37"/>
+      <c r="E68" s="37"/>
+      <c r="F68" s="37"/>
+      <c r="G68" s="37"/>
+      <c r="H68" s="37"/>
+      <c r="I68" s="37"/>
+      <c r="J68" s="37"/>
+      <c r="K68" s="37"/>
+      <c r="L68" s="37"/>
+      <c r="M68" s="37"/>
+      <c r="N68" s="37"/>
+      <c r="O68" s="37"/>
+      <c r="P68" s="37"/>
+      <c r="Q68" s="37"/>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A69" s="58" t="s">
+      <c r="A69" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="B69" s="58"/>
-      <c r="C69" s="58"/>
-      <c r="D69" s="58"/>
-      <c r="E69" s="58"/>
-      <c r="F69" s="58"/>
-      <c r="G69" s="58"/>
-      <c r="H69" s="58"/>
-      <c r="I69" s="58"/>
-      <c r="J69" s="58"/>
-      <c r="K69" s="58"/>
-      <c r="L69" s="58"/>
-      <c r="M69" s="58"/>
-      <c r="N69" s="58"/>
-      <c r="O69" s="58"/>
-      <c r="P69" s="58"/>
-      <c r="Q69" s="58"/>
+      <c r="B69" s="38"/>
+      <c r="C69" s="38"/>
+      <c r="D69" s="38"/>
+      <c r="E69" s="38"/>
+      <c r="F69" s="38"/>
+      <c r="G69" s="38"/>
+      <c r="H69" s="38"/>
+      <c r="I69" s="38"/>
+      <c r="J69" s="38"/>
+      <c r="K69" s="38"/>
+      <c r="L69" s="38"/>
+      <c r="M69" s="38"/>
+      <c r="N69" s="38"/>
+      <c r="O69" s="38"/>
+      <c r="P69" s="38"/>
+      <c r="Q69" s="38"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A70" s="59" t="s">
+      <c r="A70" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="B70" s="59"/>
-      <c r="C70" s="59"/>
-      <c r="D70" s="59"/>
-      <c r="E70" s="59"/>
-      <c r="F70" s="59"/>
-      <c r="G70" s="59"/>
-      <c r="H70" s="59"/>
-      <c r="I70" s="59"/>
-      <c r="J70" s="59"/>
-      <c r="K70" s="59"/>
-      <c r="L70" s="59"/>
-      <c r="M70" s="59"/>
-      <c r="N70" s="59"/>
-      <c r="O70" s="59"/>
-      <c r="P70" s="59"/>
-      <c r="Q70" s="59"/>
+      <c r="B70" s="39"/>
+      <c r="C70" s="39"/>
+      <c r="D70" s="39"/>
+      <c r="E70" s="39"/>
+      <c r="F70" s="39"/>
+      <c r="G70" s="39"/>
+      <c r="H70" s="39"/>
+      <c r="I70" s="39"/>
+      <c r="J70" s="39"/>
+      <c r="K70" s="39"/>
+      <c r="L70" s="39"/>
+      <c r="M70" s="39"/>
+      <c r="N70" s="39"/>
+      <c r="O70" s="39"/>
+      <c r="P70" s="39"/>
+      <c r="Q70" s="39"/>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
@@ -2611,6 +2645,261 @@
     </row>
   </sheetData>
   <mergeCells count="279">
+    <mergeCell ref="E8:K8"/>
+    <mergeCell ref="A9:Q9"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:J13"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A2:Q2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:K3"/>
+    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="E4:K4"/>
+    <mergeCell ref="E5:K5"/>
+    <mergeCell ref="E6:K6"/>
+    <mergeCell ref="E7:K7"/>
+    <mergeCell ref="K12:L13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="O12:P13"/>
+    <mergeCell ref="M17:M19"/>
+    <mergeCell ref="N17:N19"/>
+    <mergeCell ref="O17:P19"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="I17:J19"/>
+    <mergeCell ref="K17:L19"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="I14:J16"/>
+    <mergeCell ref="K14:L16"/>
+    <mergeCell ref="M14:M16"/>
+    <mergeCell ref="N14:N16"/>
+    <mergeCell ref="O14:P16"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="I20:J22"/>
+    <mergeCell ref="K20:L22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="G23:G25"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="I23:J25"/>
+    <mergeCell ref="K23:L25"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="M20:M22"/>
+    <mergeCell ref="N20:N22"/>
+    <mergeCell ref="O20:P22"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="M23:M25"/>
+    <mergeCell ref="N23:N25"/>
+    <mergeCell ref="O23:P25"/>
+    <mergeCell ref="M26:M28"/>
+    <mergeCell ref="N26:N28"/>
+    <mergeCell ref="O26:P28"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="M29:M31"/>
+    <mergeCell ref="N29:N31"/>
+    <mergeCell ref="O29:P31"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:F28"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="I29:J31"/>
+    <mergeCell ref="K29:L31"/>
+    <mergeCell ref="G26:G28"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="I26:J28"/>
+    <mergeCell ref="K26:L28"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:F34"/>
+    <mergeCell ref="G32:G34"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="I32:J34"/>
+    <mergeCell ref="K32:L34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="G35:G37"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="I35:J37"/>
+    <mergeCell ref="K35:L37"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="M32:M34"/>
+    <mergeCell ref="N32:N34"/>
+    <mergeCell ref="O32:P34"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="M35:M37"/>
+    <mergeCell ref="N35:N37"/>
+    <mergeCell ref="O35:P37"/>
+    <mergeCell ref="M38:M40"/>
+    <mergeCell ref="N38:N40"/>
+    <mergeCell ref="O38:P40"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="M41:M43"/>
+    <mergeCell ref="N41:N43"/>
+    <mergeCell ref="O41:P43"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:F40"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:F43"/>
+    <mergeCell ref="G41:G43"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="I41:J43"/>
+    <mergeCell ref="K41:L43"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="I38:J40"/>
+    <mergeCell ref="K38:L40"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="I44:J46"/>
+    <mergeCell ref="K44:L46"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="F47:F49"/>
+    <mergeCell ref="G47:G49"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="I47:J49"/>
+    <mergeCell ref="K47:L49"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="M44:M46"/>
+    <mergeCell ref="N44:N46"/>
+    <mergeCell ref="O44:P46"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="M47:M49"/>
+    <mergeCell ref="N47:N49"/>
+    <mergeCell ref="O47:P49"/>
+    <mergeCell ref="M50:M52"/>
+    <mergeCell ref="N50:N52"/>
+    <mergeCell ref="O50:P52"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="M53:M55"/>
+    <mergeCell ref="N53:N55"/>
+    <mergeCell ref="O53:P55"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="C50:C52"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:F52"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="G53:G55"/>
+    <mergeCell ref="H53:H55"/>
+    <mergeCell ref="I53:J55"/>
+    <mergeCell ref="K53:L55"/>
+    <mergeCell ref="G50:G52"/>
+    <mergeCell ref="H50:H52"/>
+    <mergeCell ref="I50:J52"/>
+    <mergeCell ref="K50:L52"/>
+    <mergeCell ref="A68:Q68"/>
+    <mergeCell ref="A69:Q69"/>
+    <mergeCell ref="A70:Q70"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="C56:C58"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="F56:F58"/>
+    <mergeCell ref="G56:G58"/>
+    <mergeCell ref="H56:H58"/>
+    <mergeCell ref="I56:J58"/>
+    <mergeCell ref="K56:L58"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="M59:M61"/>
+    <mergeCell ref="N59:N61"/>
+    <mergeCell ref="O59:P61"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="M56:M58"/>
+    <mergeCell ref="N56:N58"/>
+    <mergeCell ref="O56:P58"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="G62:G64"/>
+    <mergeCell ref="H62:H64"/>
+    <mergeCell ref="I62:J64"/>
+    <mergeCell ref="K62:L64"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="F59:F61"/>
+    <mergeCell ref="G59:G61"/>
+    <mergeCell ref="H59:H61"/>
+    <mergeCell ref="I59:J61"/>
+    <mergeCell ref="K59:L61"/>
     <mergeCell ref="M62:M64"/>
     <mergeCell ref="N62:N64"/>
     <mergeCell ref="O62:P64"/>
@@ -2635,261 +2924,6 @@
     <mergeCell ref="C62:C64"/>
     <mergeCell ref="D62:E62"/>
     <mergeCell ref="F62:F64"/>
-    <mergeCell ref="G62:G64"/>
-    <mergeCell ref="H62:H64"/>
-    <mergeCell ref="I62:J64"/>
-    <mergeCell ref="K62:L64"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="C59:C61"/>
-    <mergeCell ref="F59:F61"/>
-    <mergeCell ref="G59:G61"/>
-    <mergeCell ref="H59:H61"/>
-    <mergeCell ref="I59:J61"/>
-    <mergeCell ref="K59:L61"/>
-    <mergeCell ref="M59:M61"/>
-    <mergeCell ref="N59:N61"/>
-    <mergeCell ref="O59:P61"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="M56:M58"/>
-    <mergeCell ref="N56:N58"/>
-    <mergeCell ref="O56:P58"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="A68:Q68"/>
-    <mergeCell ref="A69:Q69"/>
-    <mergeCell ref="A70:Q70"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="C56:C58"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="F56:F58"/>
-    <mergeCell ref="G56:G58"/>
-    <mergeCell ref="H56:H58"/>
-    <mergeCell ref="I56:J58"/>
-    <mergeCell ref="K56:L58"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="M53:M55"/>
-    <mergeCell ref="N53:N55"/>
-    <mergeCell ref="O53:P55"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="C50:C52"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:F52"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="G53:G55"/>
-    <mergeCell ref="H53:H55"/>
-    <mergeCell ref="I53:J55"/>
-    <mergeCell ref="K53:L55"/>
-    <mergeCell ref="G50:G52"/>
-    <mergeCell ref="H50:H52"/>
-    <mergeCell ref="I50:J52"/>
-    <mergeCell ref="K50:L52"/>
-    <mergeCell ref="M44:M46"/>
-    <mergeCell ref="N44:N46"/>
-    <mergeCell ref="O44:P46"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="M47:M49"/>
-    <mergeCell ref="N47:N49"/>
-    <mergeCell ref="O47:P49"/>
-    <mergeCell ref="M50:M52"/>
-    <mergeCell ref="N50:N52"/>
-    <mergeCell ref="O50:P52"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="F47:F49"/>
-    <mergeCell ref="G47:G49"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="I47:J49"/>
-    <mergeCell ref="K47:L49"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="G44:G46"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="I44:J46"/>
-    <mergeCell ref="K44:L46"/>
-    <mergeCell ref="M41:M43"/>
-    <mergeCell ref="N41:N43"/>
-    <mergeCell ref="O41:P43"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F38:F40"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:F43"/>
-    <mergeCell ref="G41:G43"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="I41:J43"/>
-    <mergeCell ref="K41:L43"/>
-    <mergeCell ref="G38:G40"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="I38:J40"/>
-    <mergeCell ref="K38:L40"/>
-    <mergeCell ref="M32:M34"/>
-    <mergeCell ref="N32:N34"/>
-    <mergeCell ref="O32:P34"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="M35:M37"/>
-    <mergeCell ref="N35:N37"/>
-    <mergeCell ref="O35:P37"/>
-    <mergeCell ref="M38:M40"/>
-    <mergeCell ref="N38:N40"/>
-    <mergeCell ref="O38:P40"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="G35:G37"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="I35:J37"/>
-    <mergeCell ref="K35:L37"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:F34"/>
-    <mergeCell ref="G32:G34"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="I32:J34"/>
-    <mergeCell ref="K32:L34"/>
-    <mergeCell ref="M29:M31"/>
-    <mergeCell ref="N29:N31"/>
-    <mergeCell ref="O29:P31"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:F28"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="G29:G31"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="I29:J31"/>
-    <mergeCell ref="K29:L31"/>
-    <mergeCell ref="G26:G28"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="I26:J28"/>
-    <mergeCell ref="K26:L28"/>
-    <mergeCell ref="M20:M22"/>
-    <mergeCell ref="N20:N22"/>
-    <mergeCell ref="O20:P22"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="M23:M25"/>
-    <mergeCell ref="N23:N25"/>
-    <mergeCell ref="O23:P25"/>
-    <mergeCell ref="M26:M28"/>
-    <mergeCell ref="N26:N28"/>
-    <mergeCell ref="O26:P28"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="G23:G25"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="I23:J25"/>
-    <mergeCell ref="K23:L25"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="G20:G22"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="I20:J22"/>
-    <mergeCell ref="K20:L22"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="K12:L13"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="O12:P13"/>
-    <mergeCell ref="M17:M19"/>
-    <mergeCell ref="N17:N19"/>
-    <mergeCell ref="O17:P19"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="I17:J19"/>
-    <mergeCell ref="K17:L19"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="I14:J16"/>
-    <mergeCell ref="K14:L16"/>
-    <mergeCell ref="M14:M16"/>
-    <mergeCell ref="N14:N16"/>
-    <mergeCell ref="O14:P16"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="A2:Q2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:K3"/>
-    <mergeCell ref="L3:O3"/>
-    <mergeCell ref="E4:K4"/>
-    <mergeCell ref="E5:K5"/>
-    <mergeCell ref="E6:K6"/>
-    <mergeCell ref="E7:K7"/>
-    <mergeCell ref="E8:K8"/>
-    <mergeCell ref="A9:Q9"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:J13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F14" r:id="rId1" xr:uid="{4BD3620A-17CE-43E4-9BC7-058922B7BB43}"/>

</xml_diff>